<commit_message>
New data, plotting/stats code, table, and figure updates.
</commit_message>
<xml_diff>
--- a/tables/Table_S1.xlsx
+++ b/tables/Table_S1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="412">
   <si>
     <t>UNITE</t>
   </si>
@@ -58,28 +58,28 @@
     <t>BLAST</t>
   </si>
   <si>
-    <t>20.3±0.7 (F)</t>
-  </si>
-  <si>
-    <t>26.4±0.8 (I)</t>
+    <t>20.3±0.7 (G)</t>
+  </si>
+  <si>
+    <t>26.4±0.8 (J)</t>
   </si>
   <si>
     <t>5.1±0.6 (H)</t>
   </si>
   <si>
-    <t>40.3±1.4 (F)</t>
-  </si>
-  <si>
-    <t>54.2±2.1 (I)</t>
+    <t>40.3±1.4 (G)</t>
+  </si>
+  <si>
+    <t>54.2±2.1 (J)</t>
   </si>
   <si>
     <t>5.7±0.8 (H)</t>
   </si>
   <si>
-    <t>37.9±1.9 (F)</t>
-  </si>
-  <si>
-    <t>50.4±2.6 (I)</t>
+    <t>37.9±1.9 (G)</t>
+  </si>
+  <si>
+    <t>50.4±2.6 (J)</t>
   </si>
   <si>
     <t>6.7±1.5 (H)</t>
@@ -91,7 +91,7 @@
     <t>26.4±1.8 (A)</t>
   </si>
   <si>
-    <t>26.5±6.5 (E)</t>
+    <t>26.5±6.5 (F)</t>
   </si>
   <si>
     <t>27.9±1.2 (B)</t>
@@ -100,7 +100,7 @@
     <t>31.2±1 (A)</t>
   </si>
   <si>
-    <t>20.8±4 (E)</t>
+    <t>20.8±4 (F)</t>
   </si>
   <si>
     <t>28.6±2.7 (B)</t>
@@ -109,7 +109,7 @@
     <t>33.1±3.5 (A)</t>
   </si>
   <si>
-    <t>18.8±4.1 (E)</t>
+    <t>18.8±4.1 (F)</t>
   </si>
   <si>
     <t>RDP</t>
@@ -118,7 +118,7 @@
     <t>23.4±1.2 (D)</t>
   </si>
   <si>
-    <t>30.3±1.7 (E)</t>
+    <t>30.3±1.7 (F)</t>
   </si>
   <si>
     <t>6.2±0.8 (E)</t>
@@ -127,7 +127,7 @@
     <t>32.4±1.6 (D)</t>
   </si>
   <si>
-    <t>44.2±2.3 (E)</t>
+    <t>44.2±2.3 (F)</t>
   </si>
   <si>
     <t>2.9±0.5 (E)</t>
@@ -136,7 +136,7 @@
     <t>30.7±2.1 (D)</t>
   </si>
   <si>
-    <t>41.6±2.8 (E)</t>
+    <t>41.6±2.8 (F)</t>
   </si>
   <si>
     <t>3.2±0.7 (E)</t>
@@ -175,7 +175,7 @@
     <t>23.7±1 (B)</t>
   </si>
   <si>
-    <t>32.3±1.5 (C)</t>
+    <t>32.3±1.5 (D)</t>
   </si>
   <si>
     <t>2.1±0.4 (D)</t>
@@ -184,7 +184,7 @@
     <t>28.5±1.4 (B)</t>
   </si>
   <si>
-    <t>39±1.9 (C)</t>
+    <t>39±1.9 (D)</t>
   </si>
   <si>
     <t>2.3±0.3 (D)</t>
@@ -193,7 +193,7 @@
     <t>26.3±1.7 (B)</t>
   </si>
   <si>
-    <t>35.7±2.1 (C)</t>
+    <t>35.7±2.1 (D)</t>
   </si>
   <si>
     <t>2.7±0.8 (D)</t>
@@ -229,28 +229,28 @@
     <t>UTAX</t>
   </si>
   <si>
-    <t>31.1±2 (H)</t>
-  </si>
-  <si>
-    <t>43.2±2.8 (K)</t>
+    <t>31.1±2 (I)</t>
+  </si>
+  <si>
+    <t>43.2±2.8 (L)</t>
   </si>
   <si>
     <t>0.7±0.1 (A)</t>
   </si>
   <si>
-    <t>38.7±0.9 (H)</t>
-  </si>
-  <si>
-    <t>53.8±1.3 (K)</t>
+    <t>38.7±0.9 (I)</t>
+  </si>
+  <si>
+    <t>53.8±1.3 (L)</t>
   </si>
   <si>
     <t>1±0.1 (A)</t>
   </si>
   <si>
-    <t>36.4±1.6 (H)</t>
-  </si>
-  <si>
-    <t>50.4±2.2 (K)</t>
+    <t>36.4±1.6 (I)</t>
+  </si>
+  <si>
+    <t>50.4±2.2 (L)</t>
   </si>
   <si>
     <t>1.2±0.2 (A)</t>
@@ -259,28 +259,28 @@
     <t>mothur-wang</t>
   </si>
   <si>
-    <t>30.2±2.4 (I)</t>
-  </si>
-  <si>
-    <t>39±2.6 (J)</t>
+    <t>30.2±2.4 (J)</t>
+  </si>
+  <si>
+    <t>39±2.6 (K)</t>
   </si>
   <si>
     <t>7.9±2 (F)</t>
   </si>
   <si>
-    <t>40.4±1.7 (I)</t>
-  </si>
-  <si>
-    <t>55.5±2.4 (J)</t>
+    <t>40.4±1.7 (J)</t>
+  </si>
+  <si>
+    <t>55.5±2.4 (K)</t>
   </si>
   <si>
     <t>2.7±0.8 (F)</t>
   </si>
   <si>
-    <t>37.6±1.7 (I)</t>
-  </si>
-  <si>
-    <t>51.1±2.7 (J)</t>
+    <t>37.6±1.7 (J)</t>
+  </si>
+  <si>
+    <t>51.1±2.7 (K)</t>
   </si>
   <si>
     <t>3.7±1 (F)</t>
@@ -316,28 +316,28 @@
     <t>mothur-knn=3</t>
   </si>
   <si>
-    <t>28.7±2.6 (E)</t>
-  </si>
-  <si>
-    <t>36.6±3.6 (F)</t>
+    <t>28.7±2.6 (F)</t>
+  </si>
+  <si>
+    <t>36.6±3.6 (G)</t>
   </si>
   <si>
     <t>9±1.9 (I)</t>
   </si>
   <si>
-    <t>32.3±1.8 (E)</t>
-  </si>
-  <si>
-    <t>41.7±2.6 (F)</t>
+    <t>32.3±1.8 (F)</t>
+  </si>
+  <si>
+    <t>41.7±2.6 (G)</t>
   </si>
   <si>
     <t>8.6±1.1 (I)</t>
   </si>
   <si>
-    <t>30.6±2.5 (E)</t>
-  </si>
-  <si>
-    <t>39.3±3.2 (F)</t>
+    <t>30.6±2.5 (F)</t>
+  </si>
+  <si>
+    <t>39.3±3.2 (G)</t>
   </si>
   <si>
     <t>8.9±1.8 (I)</t>
@@ -373,58 +373,145 @@
     <t>qiime2-Naive-Bayes</t>
   </si>
   <si>
-    <t>32.2±2.6 (G)</t>
-  </si>
-  <si>
-    <t>36.3±2.9 (H)</t>
-  </si>
-  <si>
-    <t>21.8±2.9 (K)</t>
-  </si>
-  <si>
-    <t>36.1±1.2 (G)</t>
-  </si>
-  <si>
-    <t>44.5±2.2 (H)</t>
-  </si>
-  <si>
-    <t>15.3±1.8 (K)</t>
-  </si>
-  <si>
-    <t>35.1±1.2 (G)</t>
-  </si>
-  <si>
-    <t>41.6±3 (H)</t>
-  </si>
-  <si>
-    <t>18.9±3.5 (K)</t>
-  </si>
-  <si>
-    <t>66.3±20.4 (E)</t>
+    <t>32.2±2.6 (H)</t>
+  </si>
+  <si>
+    <t>36.3±2.9 (I)</t>
+  </si>
+  <si>
+    <t>21.8±2.9 (L)</t>
+  </si>
+  <si>
+    <t>36.1±1.2 (H)</t>
+  </si>
+  <si>
+    <t>44.5±2.2 (I)</t>
+  </si>
+  <si>
+    <t>15.3±1.8 (L)</t>
+  </si>
+  <si>
+    <t>35.1±1.2 (H)</t>
+  </si>
+  <si>
+    <t>41.6±3 (I)</t>
+  </si>
+  <si>
+    <t>18.9±3.5 (L)</t>
+  </si>
+  <si>
+    <t>66.3±20.4 (F)</t>
   </si>
   <si>
     <t>66.6±22.4 (F)</t>
   </si>
   <si>
-    <t>65.6±23.8 (G)</t>
-  </si>
-  <si>
-    <t>31.3±2.1 (E)</t>
+    <t>65.6±23.8 (H)</t>
+  </si>
+  <si>
+    <t>31.3±2.1 (F)</t>
   </si>
   <si>
     <t>33.2±4 (F)</t>
   </si>
   <si>
-    <t>26.6±5.6 (G)</t>
-  </si>
-  <si>
-    <t>29.6±2 (E)</t>
+    <t>26.6±5.6 (H)</t>
+  </si>
+  <si>
+    <t>29.6±2 (F)</t>
   </si>
   <si>
     <t>32.7±2 (F)</t>
   </si>
   <si>
-    <t>21.8±3.4 (G)</t>
+    <t>21.8±3.4 (H)</t>
+  </si>
+  <si>
+    <t>Kraken2</t>
+  </si>
+  <si>
+    <t>27.1±0.8 (E)</t>
+  </si>
+  <si>
+    <t>6.1±0.8 (A)</t>
+  </si>
+  <si>
+    <t>79.6±1.9 (M)</t>
+  </si>
+  <si>
+    <t>32.3±1.5 (E)</t>
+  </si>
+  <si>
+    <t>18.6±2.4 (A)</t>
+  </si>
+  <si>
+    <t>66.4±2.3 (M)</t>
+  </si>
+  <si>
+    <t>30.4±1.4 (E)</t>
+  </si>
+  <si>
+    <t>15.2±1.9 (A)</t>
+  </si>
+  <si>
+    <t>68.5±2.2 (M)</t>
+  </si>
+  <si>
+    <t>70.3±0.1 (E)</t>
+  </si>
+  <si>
+    <t>98.3±0.2 (G)</t>
+  </si>
+  <si>
+    <t>0.1±0.1 (E)</t>
+  </si>
+  <si>
+    <t>20.5±1.3 (E)</t>
+  </si>
+  <si>
+    <t>17.2±1.2 (G)</t>
+  </si>
+  <si>
+    <t>29±2.3 (E)</t>
+  </si>
+  <si>
+    <t>22.1±2.1 (E)</t>
+  </si>
+  <si>
+    <t>20.8±2.3 (G)</t>
+  </si>
+  <si>
+    <t>25.4±2.9 (E)</t>
+  </si>
+  <si>
+    <t>SPINGO</t>
+  </si>
+  <si>
+    <t>28.3±1.5 (K)</t>
+  </si>
+  <si>
+    <t>31.1±2 (M)</t>
+  </si>
+  <si>
+    <t>21.3±1.4 (K)</t>
+  </si>
+  <si>
+    <t>63.7±3.7 (K)</t>
+  </si>
+  <si>
+    <t>88.2±5.6 (M)</t>
+  </si>
+  <si>
+    <t>2.4±1.2 (K)</t>
+  </si>
+  <si>
+    <t>43.7±9.5 (K)</t>
+  </si>
+  <si>
+    <t>56.5±13.7 (M)</t>
+  </si>
+  <si>
+    <t>11.5±1.4 (K)</t>
   </si>
   <si>
     <t>CB</t>
@@ -433,7 +520,7 @@
     <t>20.8±0.5 (A)</t>
   </si>
   <si>
-    <t>24.8±0.6 (A)</t>
+    <t>24.8±0.6 (B)</t>
   </si>
   <si>
     <t>10.7±0.8 (J)</t>
@@ -442,7 +529,7 @@
     <t>28.8±1.1 (A)</t>
   </si>
   <si>
-    <t>36.9±1.7 (A)</t>
+    <t>36.9±1.7 (B)</t>
   </si>
   <si>
     <t>8.4±0.7 (J)</t>
@@ -451,7 +538,7 @@
     <t>27.2±1.8 (A)</t>
   </si>
   <si>
-    <t>34.3±1.9 (A)</t>
+    <t>34.3±1.9 (B)</t>
   </si>
   <si>
     <t>9.6±2 (J)</t>
@@ -463,7 +550,7 @@
     <t>26.7±2.2 (A)</t>
   </si>
   <si>
-    <t>35.2±8.5 (F)</t>
+    <t>35.2±8.5 (G)</t>
   </si>
   <si>
     <t>29.1±3.4 (C)</t>
@@ -472,7 +559,7 @@
     <t>32.2±2.7 (A)</t>
   </si>
   <si>
-    <t>21.6±15.3 (F)</t>
+    <t>21.6±15.3 (G)</t>
   </si>
   <si>
     <t>28.5±3.3 (C)</t>
@@ -481,7 +568,7 @@
     <t>32.8±2.5 (A)</t>
   </si>
   <si>
-    <t>18.7±13 (F)</t>
+    <t>18.7±13 (G)</t>
   </si>
   <si>
     <t>CBC</t>
@@ -490,181 +577,184 @@
     <t>21.4±0.8 (C)</t>
   </si>
   <si>
+    <t>29.2±1.1 (E)</t>
+  </si>
+  <si>
+    <t>2±0.2 (C)</t>
+  </si>
+  <si>
+    <t>31±1.6 (C)</t>
+  </si>
+  <si>
+    <t>42.6±2.2 (E)</t>
+  </si>
+  <si>
+    <t>1.9±0.4 (C)</t>
+  </si>
+  <si>
+    <t>29.1±1.8 (C)</t>
+  </si>
+  <si>
+    <t>39.8±2.4 (E)</t>
+  </si>
+  <si>
+    <t>2.2±0.5 (C)</t>
+  </si>
+  <si>
+    <t>20.9±2.5 (A)</t>
+  </si>
+  <si>
+    <t>28.3±2 (B)</t>
+  </si>
+  <si>
+    <t>3.7±1.5 (A)</t>
+  </si>
+  <si>
+    <t>26±2.5 (A)</t>
+  </si>
+  <si>
+    <t>34.9±3 (B)</t>
+  </si>
+  <si>
+    <t>5.6±1.7 (A)</t>
+  </si>
+  <si>
+    <t>25.3±1.8 (A)</t>
+  </si>
+  <si>
+    <t>34.4±2.6 (B)</t>
+  </si>
+  <si>
+    <t>4.8±1.3 (A)</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>22±0.6 (A)</t>
+  </si>
+  <si>
+    <t>28.1±0.9 (C)</t>
+  </si>
+  <si>
+    <t>6.8±0.9 (G)</t>
+  </si>
+  <si>
+    <t>28.5±1.4 (A)</t>
+  </si>
+  <si>
+    <t>38.4±1.9 (C)</t>
+  </si>
+  <si>
+    <t>4±0.5 (G)</t>
+  </si>
+  <si>
+    <t>26.6±1.8 (A)</t>
+  </si>
+  <si>
+    <t>35.4±2.1 (C)</t>
+  </si>
+  <si>
+    <t>4.5±1.2 (G)</t>
+  </si>
+  <si>
+    <t>CUC</t>
+  </si>
+  <si>
+    <t>24.3±1.2 (D)</t>
+  </si>
+  <si>
+    <t>33.4±1.8 (H)</t>
+  </si>
+  <si>
+    <t>1.6±0.3 (B)</t>
+  </si>
+  <si>
+    <t>32.1±1.5 (D)</t>
+  </si>
+  <si>
+    <t>44.3±2.2 (H)</t>
+  </si>
+  <si>
+    <t>30.2±2 (D)</t>
+  </si>
+  <si>
+    <t>41.5±2.7 (H)</t>
+  </si>
+  <si>
+    <t>1.8±0.4 (B)</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>19±0.8 (G)</t>
+  </si>
+  <si>
+    <t>22±1 (G)</t>
+  </si>
+  <si>
+    <t>0.6±0.2 (C)</t>
+  </si>
+  <si>
+    <t>35.1±1.8 (G)</t>
+  </si>
+  <si>
+    <t>40.3±2 (G)</t>
+  </si>
+  <si>
+    <t>4.2±0.4 (C)</t>
+  </si>
+  <si>
+    <t>30.7±1.9 (G)</t>
+  </si>
+  <si>
+    <t>35.3±2.2 (G)</t>
+  </si>
+  <si>
+    <t>3.5±0.4 (C)</t>
+  </si>
+  <si>
+    <t>22.6±1.2 (B)</t>
+  </si>
+  <si>
+    <t>22.7±1.7 (A)</t>
+  </si>
+  <si>
+    <t>22.4±2.6 (F)</t>
+  </si>
+  <si>
+    <t>23.7±1.7 (B)</t>
+  </si>
+  <si>
+    <t>24±1.9 (A)</t>
+  </si>
+  <si>
+    <t>21.9±6.1 (F)</t>
+  </si>
+  <si>
+    <t>25.9±1.4 (B)</t>
+  </si>
+  <si>
+    <t>27.2±1.4 (A)</t>
+  </si>
+  <si>
+    <t>18.4±4.5 (F)</t>
+  </si>
+  <si>
+    <t>21.2±0.8 (D)</t>
+  </si>
+  <si>
+    <t>23.2±0.8 (E)</t>
+  </si>
+  <si>
+    <t>9.2±0.8 (D)</t>
+  </si>
+  <si>
     <t>29.2±1.1 (D)</t>
   </si>
   <si>
-    <t>2±0.2 (C)</t>
-  </si>
-  <si>
-    <t>31±1.6 (C)</t>
-  </si>
-  <si>
-    <t>42.6±2.2 (D)</t>
-  </si>
-  <si>
-    <t>1.9±0.4 (C)</t>
-  </si>
-  <si>
-    <t>29.1±1.8 (C)</t>
-  </si>
-  <si>
-    <t>39.8±2.4 (D)</t>
-  </si>
-  <si>
-    <t>2.2±0.5 (C)</t>
-  </si>
-  <si>
-    <t>20.9±2.5 (A)</t>
-  </si>
-  <si>
-    <t>28.3±2 (B)</t>
-  </si>
-  <si>
-    <t>3.7±1.5 (A)</t>
-  </si>
-  <si>
-    <t>26±2.5 (A)</t>
-  </si>
-  <si>
-    <t>34.9±3 (B)</t>
-  </si>
-  <si>
-    <t>5.6±1.7 (A)</t>
-  </si>
-  <si>
-    <t>25.3±1.8 (A)</t>
-  </si>
-  <si>
-    <t>34.4±2.6 (B)</t>
-  </si>
-  <si>
-    <t>4.8±1.3 (A)</t>
-  </si>
-  <si>
-    <t>CU</t>
-  </si>
-  <si>
-    <t>22±0.6 (A)</t>
-  </si>
-  <si>
-    <t>28.1±0.9 (B)</t>
-  </si>
-  <si>
-    <t>6.8±0.9 (G)</t>
-  </si>
-  <si>
-    <t>28.5±1.4 (A)</t>
-  </si>
-  <si>
-    <t>38.4±1.9 (B)</t>
-  </si>
-  <si>
-    <t>4±0.5 (G)</t>
-  </si>
-  <si>
-    <t>26.6±1.8 (A)</t>
-  </si>
-  <si>
-    <t>35.4±2.1 (B)</t>
-  </si>
-  <si>
-    <t>4.5±1.2 (G)</t>
-  </si>
-  <si>
-    <t>CUC</t>
-  </si>
-  <si>
-    <t>24.3±1.2 (D)</t>
-  </si>
-  <si>
-    <t>33.4±1.8 (G)</t>
-  </si>
-  <si>
-    <t>1.6±0.3 (B)</t>
-  </si>
-  <si>
-    <t>32.1±1.5 (D)</t>
-  </si>
-  <si>
-    <t>44.3±2.2 (G)</t>
-  </si>
-  <si>
-    <t>30.2±2 (D)</t>
-  </si>
-  <si>
-    <t>41.5±2.7 (G)</t>
-  </si>
-  <si>
-    <t>1.8±0.4 (B)</t>
-  </si>
-  <si>
-    <t>gen</t>
-  </si>
-  <si>
-    <t>19±0.8 (F)</t>
-  </si>
-  <si>
-    <t>22±1 (F)</t>
-  </si>
-  <si>
-    <t>0.6±0.2 (C)</t>
-  </si>
-  <si>
-    <t>35.1±1.8 (F)</t>
-  </si>
-  <si>
-    <t>40.3±2 (F)</t>
-  </si>
-  <si>
-    <t>4.2±0.4 (C)</t>
-  </si>
-  <si>
-    <t>30.7±1.9 (F)</t>
-  </si>
-  <si>
-    <t>35.3±2.2 (F)</t>
-  </si>
-  <si>
-    <t>3.5±0.4 (C)</t>
-  </si>
-  <si>
-    <t>22.6±1.2 (B)</t>
-  </si>
-  <si>
-    <t>22.7±1.7 (A)</t>
-  </si>
-  <si>
-    <t>22.4±2.6 (F)</t>
-  </si>
-  <si>
-    <t>23.7±1.7 (B)</t>
-  </si>
-  <si>
-    <t>24±1.9 (A)</t>
-  </si>
-  <si>
-    <t>21.9±6.1 (F)</t>
-  </si>
-  <si>
-    <t>25.9±1.4 (B)</t>
-  </si>
-  <si>
-    <t>27.2±1.4 (A)</t>
-  </si>
-  <si>
-    <t>18.4±4.5 (F)</t>
-  </si>
-  <si>
-    <t>21.2±0.8 (D)</t>
-  </si>
-  <si>
-    <t>23.2±0.8 (D)</t>
-  </si>
-  <si>
-    <t>9.2±0.8 (D)</t>
-  </si>
-  <si>
-    <t>33.3±1.3 (D)</t>
+    <t>33.3±1.3 (E)</t>
   </si>
   <si>
     <t>4.7±0.5 (D)</t>
@@ -673,7 +763,7 @@
     <t>26.2±1.3 (D)</t>
   </si>
   <si>
-    <t>29.8±1.3 (D)</t>
+    <t>29.8±1.3 (E)</t>
   </si>
   <si>
     <t>4.7±1 (D)</t>
@@ -709,22 +799,22 @@
     <t>22.6±0.9 (C)</t>
   </si>
   <si>
-    <t>26.3±1 (C)</t>
-  </si>
-  <si>
-    <t>0±0 (ABCDEF)</t>
+    <t>26.3±1 (D)</t>
+  </si>
+  <si>
+    <t>0±0 (ABCDEFGH)</t>
   </si>
   <si>
     <t>26.2±0.8 (C)</t>
   </si>
   <si>
-    <t>30.6±1 (C)</t>
+    <t>30.6±1 (D)</t>
   </si>
   <si>
     <t>23.4±1 (C)</t>
   </si>
   <si>
-    <t>27.2±1.1 (C)</t>
+    <t>27.2±1.1 (D)</t>
   </si>
   <si>
     <t>25.1±1.3 (D)</t>
@@ -748,52 +838,52 @@
     <t>33.7±1.6 (E)</t>
   </si>
   <si>
-    <t>34.3±1.8 (G)</t>
-  </si>
-  <si>
-    <t>39.9±2.1 (G)</t>
+    <t>34.3±1.8 (H)</t>
+  </si>
+  <si>
+    <t>39.9±2.1 (H)</t>
   </si>
   <si>
     <t>0.4±0.1 (A)</t>
   </si>
   <si>
-    <t>39.7±1.2 (G)</t>
-  </si>
-  <si>
-    <t>46.3±1.4 (G)</t>
+    <t>39.7±1.2 (H)</t>
+  </si>
+  <si>
+    <t>46.3±1.4 (H)</t>
   </si>
   <si>
     <t>0.7±0.2 (A)</t>
   </si>
   <si>
-    <t>36.6±1.1 (G)</t>
-  </si>
-  <si>
-    <t>42.6±1.3 (G)</t>
-  </si>
-  <si>
-    <t>38.9±1.9 (J)</t>
-  </si>
-  <si>
-    <t>43.2±1.8 (J)</t>
+    <t>36.6±1.1 (H)</t>
+  </si>
+  <si>
+    <t>42.6±1.3 (H)</t>
+  </si>
+  <si>
+    <t>38.9±1.9 (K)</t>
+  </si>
+  <si>
+    <t>43.2±1.8 (K)</t>
   </si>
   <si>
     <t>13±4.5 (E)</t>
   </si>
   <si>
-    <t>48.5±2.9 (J)</t>
-  </si>
-  <si>
-    <t>55.7±3.5 (J)</t>
+    <t>48.5±2.9 (K)</t>
+  </si>
+  <si>
+    <t>55.7±3.5 (K)</t>
   </si>
   <si>
     <t>5.4±1.2 (E)</t>
   </si>
   <si>
-    <t>46.5±1.4 (J)</t>
-  </si>
-  <si>
-    <t>53.1±1.7 (J)</t>
+    <t>46.5±1.4 (K)</t>
+  </si>
+  <si>
+    <t>53.1±1.7 (K)</t>
   </si>
   <si>
     <t>6.5±0.5 (E)</t>
@@ -826,28 +916,28 @@
     <t>7.5±4.3 (B)</t>
   </si>
   <si>
-    <t>35.7±1.9 (H)</t>
-  </si>
-  <si>
-    <t>41.4±2.4 (H)</t>
+    <t>35.7±1.9 (I)</t>
+  </si>
+  <si>
+    <t>41.4±2.4 (I)</t>
   </si>
   <si>
     <t>1.5±1.3 (B)</t>
   </si>
   <si>
-    <t>39±2.2 (H)</t>
-  </si>
-  <si>
-    <t>45.2±2.8 (H)</t>
+    <t>39±2.2 (I)</t>
+  </si>
+  <si>
+    <t>45.2±2.8 (I)</t>
   </si>
   <si>
     <t>2±1.8 (B)</t>
   </si>
   <si>
-    <t>38.5±2.3 (H)</t>
-  </si>
-  <si>
-    <t>44.5±2.8 (H)</t>
+    <t>38.5±2.3 (I)</t>
+  </si>
+  <si>
+    <t>44.5±2.8 (I)</t>
   </si>
   <si>
     <t>2.2±2 (B)</t>
@@ -880,31 +970,31 @@
     <t>12.6±4 (C)</t>
   </si>
   <si>
-    <t>38.1±1.9 (I)</t>
-  </si>
-  <si>
-    <t>40.5±1.9 (I)</t>
-  </si>
-  <si>
-    <t>23.5±4.7 (F)</t>
-  </si>
-  <si>
-    <t>47.8±9 (I)</t>
-  </si>
-  <si>
-    <t>53.4±11.8 (I)</t>
-  </si>
-  <si>
-    <t>14.1±8.6 (F)</t>
-  </si>
-  <si>
-    <t>42±2 (I)</t>
-  </si>
-  <si>
-    <t>45.7±2.2 (I)</t>
-  </si>
-  <si>
-    <t>19.8±2.5 (F)</t>
+    <t>38.1±1.9 (J)</t>
+  </si>
+  <si>
+    <t>40.5±1.9 (J)</t>
+  </si>
+  <si>
+    <t>23.5±4.7 (G)</t>
+  </si>
+  <si>
+    <t>47.8±9 (J)</t>
+  </si>
+  <si>
+    <t>53.4±11.8 (J)</t>
+  </si>
+  <si>
+    <t>14.1±8.6 (G)</t>
+  </si>
+  <si>
+    <t>42±2 (J)</t>
+  </si>
+  <si>
+    <t>45.7±2.2 (J)</t>
+  </si>
+  <si>
+    <t>19.8±2.5 (G)</t>
   </si>
   <si>
     <t>37±22.6 (F)</t>
@@ -934,10 +1024,82 @@
     <t>15.4±4.5 (G)</t>
   </si>
   <si>
+    <t>20.8±2.4 (F)</t>
+  </si>
+  <si>
+    <t>14.8±4.5 (A)</t>
+  </si>
+  <si>
+    <t>56.9±10.6 (H)</t>
+  </si>
+  <si>
+    <t>31±6.1 (F)</t>
+  </si>
+  <si>
+    <t>28.5±9.3 (A)</t>
+  </si>
+  <si>
+    <t>46.3±13.1 (H)</t>
+  </si>
+  <si>
+    <t>27.9±5.1 (F)</t>
+  </si>
+  <si>
+    <t>24.7±7.9 (A)</t>
+  </si>
+  <si>
+    <t>47.5±12.3 (H)</t>
+  </si>
+  <si>
+    <t>84.6±0.2 (H)</t>
+  </si>
+  <si>
+    <t>98.7±0.2 (G)</t>
+  </si>
+  <si>
+    <t>23.3±3.3 (H)</t>
+  </si>
+  <si>
+    <t>27.2±3.8 (G)</t>
+  </si>
+  <si>
+    <t>26.6±2.6 (H)</t>
+  </si>
+  <si>
+    <t>31±3 (G)</t>
+  </si>
+  <si>
+    <t>42.1±11.8 (L)</t>
+  </si>
+  <si>
+    <t>44.7±15.4 (L)</t>
+  </si>
+  <si>
+    <t>26.7±9.9 (F)</t>
+  </si>
+  <si>
+    <t>78.9±7.8 (L)</t>
+  </si>
+  <si>
+    <t>91.8±9.7 (L)</t>
+  </si>
+  <si>
+    <t>2±3.9 (F)</t>
+  </si>
+  <si>
+    <t>48.9±11.4 (L)</t>
+  </si>
+  <si>
+    <t>54.3±14 (L)</t>
+  </si>
+  <si>
+    <t>16.3±4.5 (F)</t>
+  </si>
+  <si>
     <t>18.9±0.7 (A)</t>
   </si>
   <si>
-    <t>20.4±0.7 (A)</t>
+    <t>20.4±0.7 (B)</t>
   </si>
   <si>
     <t>9.6±0.9 (E)</t>
@@ -946,7 +1108,7 @@
     <t>25.6±1 (A)</t>
   </si>
   <si>
-    <t>28.5±1.1 (A)</t>
+    <t>28.5±1.1 (B)</t>
   </si>
   <si>
     <t>8±0.8 (E)</t>
@@ -955,7 +1117,7 @@
     <t>23±1.1 (A)</t>
   </si>
   <si>
-    <t>25.6±1.1 (A)</t>
+    <t>25.6±1.1 (B)</t>
   </si>
   <si>
     <t>7.6±1.1 (E)</t>
@@ -991,7 +1153,7 @@
     <t>20.2±0.8 (C)</t>
   </si>
   <si>
-    <t>23.5±0.9 (C)</t>
+    <t>23.5±0.9 (D)</t>
   </si>
   <si>
     <t>0.1±0 (A)</t>
@@ -1000,7 +1162,7 @@
     <t>27.8±1.1 (C)</t>
   </si>
   <si>
-    <t>32.3±1.3 (C)</t>
+    <t>32.3±1.3 (D)</t>
   </si>
   <si>
     <t>0.8±0.1 (A)</t>
@@ -1009,7 +1171,7 @@
     <t>24.7±1.2 (C)</t>
   </si>
   <si>
-    <t>28.7±1.4 (C)</t>
+    <t>28.7±1.4 (D)</t>
   </si>
   <si>
     <t>0.6±0.1 (A)</t>
@@ -1045,7 +1207,7 @@
     <t>20.9±0.8 (B)</t>
   </si>
   <si>
-    <t>22.8±0.8 (B)</t>
+    <t>22.8±0.8 (C)</t>
   </si>
   <si>
     <t>9.3±0.8 (D)</t>
@@ -1054,31 +1216,31 @@
     <t>26.4±0.9 (B)</t>
   </si>
   <si>
-    <t>30±1 (B)</t>
+    <t>30±1 (C)</t>
   </si>
   <si>
     <t>23.7±1.1 (B)</t>
   </si>
   <si>
-    <t>26.8±1.1 (B)</t>
+    <t>26.8±1.1 (C)</t>
   </si>
   <si>
     <t>22.9±0.8 (E)</t>
   </si>
   <si>
-    <t>26.6±1 (E)</t>
+    <t>26.6±1 (F)</t>
   </si>
   <si>
     <t>28.8±1.1 (E)</t>
   </si>
   <si>
-    <t>33.5±1.3 (E)</t>
+    <t>33.5±1.3 (F)</t>
   </si>
   <si>
     <t>25.8±1.2 (E)</t>
   </si>
   <si>
-    <t>30±1.4 (E)</t>
+    <t>30±1.4 (F)</t>
   </si>
   <si>
     <t>0.6±0.2 (A)</t>
@@ -1452,7 +1614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1587,7 +1749,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>356</v>
+        <v>410</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -2081,75 +2243,75 @@
       <c r="K12" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="3"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="L13" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="M13" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="N13" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="O13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="P13" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="Q13" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="R13" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="S13" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="T13" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1"/>
@@ -2172,306 +2334,306 @@
         <v>190</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="3"/>
+        <v>194</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="1" t="s">
-        <v>357</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>212</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>214</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>217</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="M16" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>229</v>
-      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="3"/>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>411</v>
+      </c>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>232</v>
       </c>
       <c r="L17" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="R17" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="S17" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="3"/>
+      <c r="M18" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="T19" s="4" t="s">
         <v>269</v>
@@ -2480,316 +2642,316 @@
     <row r="20" spans="1:20">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="L20" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="3"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="N21" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="O21" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="R21" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="S21" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="R22" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="O23" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="R23" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>335</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="R23" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="N24" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="P24" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="3"/>
+      <c r="Q24" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="1"/>
       <c r="B25" s="3" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>246</v>
+        <v>353</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>73</v>
+        <v>356</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="3"/>
@@ -2800,6 +2962,210 @@
       <c r="R25" s="4"/>
       <c r="S25" s="3"/>
       <c r="T25" s="4"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2811,8 +3177,8 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A4:A14"/>
-    <mergeCell ref="A15:A25"/>
+    <mergeCell ref="A4:A16"/>
+    <mergeCell ref="A17:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>